<commit_message>
Update LL+fading experiments' results
</commit_message>
<xml_diff>
--- a/IDA2015/PreliminaryExperiments/Test2_resultsLL.xlsx
+++ b/IDA2015/PreliminaryExperiments/Test2_resultsLL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LL" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="232">
   <si>
     <t xml:space="preserve">Window Size </t>
   </si>
@@ -427,10 +427,298 @@
     <t xml:space="preserve">WASTE INCINERATOR -  No latent variables </t>
   </si>
   <si>
-    <t xml:space="preserve">WASTE INCINERATOR -  Mout as latent   </t>
-  </si>
-  <si>
     <t xml:space="preserve">NORMAL|1NORMAL PARENT - No latent variables </t>
+  </si>
+  <si>
+    <t>SampleSize=10000</t>
+  </si>
+  <si>
+    <t>4.009 m</t>
+  </si>
+  <si>
+    <t>908.6 ms</t>
+  </si>
+  <si>
+    <t>435.7 ms</t>
+  </si>
+  <si>
+    <t>295.2 ms</t>
+  </si>
+  <si>
+    <t>172.2 ms</t>
+  </si>
+  <si>
+    <t>302.9 ms</t>
+  </si>
+  <si>
+    <t>260.8 ms</t>
+  </si>
+  <si>
+    <t>425.8 ms</t>
+  </si>
+  <si>
+    <t>435.9 ms</t>
+  </si>
+  <si>
+    <t>488.9 ms</t>
+  </si>
+  <si>
+    <t>598.8 ms</t>
+  </si>
+  <si>
+    <t>802.6 ms</t>
+  </si>
+  <si>
+    <t>986.5 ms</t>
+  </si>
+  <si>
+    <t>99.84 ms</t>
+  </si>
+  <si>
+    <t>99.96 ms</t>
+  </si>
+  <si>
+    <t>98.78 ms</t>
+  </si>
+  <si>
+    <t>94.93 ms</t>
+  </si>
+  <si>
+    <t>151.2 ms</t>
+  </si>
+  <si>
+    <t>159.0 ms</t>
+  </si>
+  <si>
+    <t>211.7 ms</t>
+  </si>
+  <si>
+    <t>361.7 ms</t>
+  </si>
+  <si>
+    <t>375.1 ms</t>
+  </si>
+  <si>
+    <t>336.2 ms</t>
+  </si>
+  <si>
+    <t>377.6 ms</t>
+  </si>
+  <si>
+    <t>695.9 ms</t>
+  </si>
+  <si>
+    <t>118.5 ms</t>
+  </si>
+  <si>
+    <t>101.7 ms</t>
+  </si>
+  <si>
+    <t>74.08 ms</t>
+  </si>
+  <si>
+    <t>76.58 ms</t>
+  </si>
+  <si>
+    <t>101.6 ms</t>
+  </si>
+  <si>
+    <t>105.9 ms</t>
+  </si>
+  <si>
+    <t>125.1 ms</t>
+  </si>
+  <si>
+    <t>154.4 ms</t>
+  </si>
+  <si>
+    <t>239.2 ms</t>
+  </si>
+  <si>
+    <t>265.2 ms</t>
+  </si>
+  <si>
+    <t>224.3 ms</t>
+  </si>
+  <si>
+    <t>269.9 ms</t>
+  </si>
+  <si>
+    <t>152.1 ms</t>
+  </si>
+  <si>
+    <t>178.0 ms</t>
+  </si>
+  <si>
+    <t>96.15 ms</t>
+  </si>
+  <si>
+    <t>93.08 ms</t>
+  </si>
+  <si>
+    <t>226.9 ms</t>
+  </si>
+  <si>
+    <t>165.1 ms</t>
+  </si>
+  <si>
+    <t>122.0 ms</t>
+  </si>
+  <si>
+    <t>310.7 ms</t>
+  </si>
+  <si>
+    <t>170.4 ms</t>
+  </si>
+  <si>
+    <t>160.2 ms</t>
+  </si>
+  <si>
+    <t>177.1 ms</t>
+  </si>
+  <si>
+    <t>228.0 ms</t>
+  </si>
+  <si>
+    <t>90.79 ms</t>
+  </si>
+  <si>
+    <t>85.81 ms</t>
+  </si>
+  <si>
+    <t>95.23 ms</t>
+  </si>
+  <si>
+    <t>87.46 ms</t>
+  </si>
+  <si>
+    <t>110.7 ms</t>
+  </si>
+  <si>
+    <t>117.8 ms</t>
+  </si>
+  <si>
+    <t>125.3 ms</t>
+  </si>
+  <si>
+    <t>125.9 ms</t>
+  </si>
+  <si>
+    <t>146.0 ms</t>
+  </si>
+  <si>
+    <t>195.1 ms</t>
+  </si>
+  <si>
+    <t>276.2 ms</t>
+  </si>
+  <si>
+    <t>435.2 ms</t>
+  </si>
+  <si>
+    <t>408.6 ms</t>
+  </si>
+  <si>
+    <t>398.9 ms</t>
+  </si>
+  <si>
+    <t>406.0 ms</t>
+  </si>
+  <si>
+    <t>453.0 ms</t>
+  </si>
+  <si>
+    <t>447.3 ms</t>
+  </si>
+  <si>
+    <t>546.4 ms</t>
+  </si>
+  <si>
+    <t>471.9 ms</t>
+  </si>
+  <si>
+    <t>486.2 ms</t>
+  </si>
+  <si>
+    <t>461.8 ms</t>
+  </si>
+  <si>
+    <t>503.7 ms</t>
+  </si>
+  <si>
+    <t>532.6 ms</t>
+  </si>
+  <si>
+    <t>2.885 s</t>
+  </si>
+  <si>
+    <t>2.606 s</t>
+  </si>
+  <si>
+    <t>2.660 s</t>
+  </si>
+  <si>
+    <t>2.697 s</t>
+  </si>
+  <si>
+    <t>2.688 s</t>
+  </si>
+  <si>
+    <t>2.564 s</t>
+  </si>
+  <si>
+    <t>2.622 s</t>
+  </si>
+  <si>
+    <t>2.870 s</t>
+  </si>
+  <si>
+    <t>2.796 s</t>
+  </si>
+  <si>
+    <t>2.614 s</t>
+  </si>
+  <si>
+    <t>2.589 s</t>
+  </si>
+  <si>
+    <t>2.800 s</t>
+  </si>
+  <si>
+    <t>4.926 s</t>
+  </si>
+  <si>
+    <t>5.216 s</t>
+  </si>
+  <si>
+    <t>5.449 s</t>
+  </si>
+  <si>
+    <t>5.260 s</t>
+  </si>
+  <si>
+    <t>5.180 s</t>
+  </si>
+  <si>
+    <t>5.270 s</t>
+  </si>
+  <si>
+    <t>5.285 s</t>
+  </si>
+  <si>
+    <t>5.242 s</t>
+  </si>
+  <si>
+    <t>5.233 s</t>
+  </si>
+  <si>
+    <t>5.626 s</t>
+  </si>
+  <si>
+    <t>6.996 s</t>
+  </si>
+  <si>
+    <t>5.899 s</t>
   </si>
 </sst>
 </file>
@@ -591,7 +879,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -639,8 +927,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -663,8 +959,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -688,6 +985,10 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -711,6 +1012,10 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1043,7 +1348,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1642,14 +1947,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK30"/>
+  <dimension ref="A1:AK22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
@@ -1718,6 +2024,9 @@
       <c r="AK1" s="5"/>
     </row>
     <row r="2" spans="1:37">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
@@ -2612,248 +2921,1150 @@
       </c>
     </row>
     <row r="11" spans="1:37">
-      <c r="A11" s="5" t="s">
+      <c r="A11">
+        <v>10000</v>
+      </c>
+      <c r="B11" s="2">
+        <v>29991.230899394199</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="10"/>
+      <c r="AI11" s="10"/>
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="10"/>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="5"/>
-      <c r="AH11" s="5"/>
-      <c r="AI11" s="5"/>
-      <c r="AJ11" s="5"/>
-      <c r="AK11" s="5"/>
-    </row>
-    <row r="12" spans="1:37">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>0.99990000000000001</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>0.999</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>0.99</v>
       </c>
-      <c r="N12">
+      <c r="N13">
         <v>0.9</v>
       </c>
-      <c r="Q12">
+      <c r="Q13">
         <v>0.8</v>
       </c>
-      <c r="T12">
+      <c r="T13">
         <v>0.7</v>
       </c>
-      <c r="W12">
+      <c r="W13">
         <v>0.6</v>
       </c>
-      <c r="Z12">
+      <c r="Z13">
         <v>0.5</v>
       </c>
-      <c r="AC12">
+      <c r="AC13">
         <v>0.4</v>
       </c>
-      <c r="AF12">
+      <c r="AF13">
         <v>0.3</v>
       </c>
-      <c r="AI12">
+      <c r="AI13">
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
-      <c r="A13" t="s">
+    <row r="14" spans="1:37">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:37">
-      <c r="A14">
-        <v>1</v>
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK14" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:37">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B15" s="7">
+        <v>-47747.957728000198</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2.0051999999999999</v>
+      </c>
+      <c r="E15" s="7">
+        <v>-47615.119469215097</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="9">
+        <v>2.0051999999999999</v>
+      </c>
+      <c r="H15" s="7">
+        <v>-45991.691288789603</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" s="9">
+        <v>2.0053999999999998</v>
+      </c>
+      <c r="K15" s="7">
+        <v>-34379.793574680101</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="M15" s="9">
+        <v>2.0369000000000002</v>
+      </c>
+      <c r="N15" s="18">
+        <v>-31470.746630448401</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="P15" s="9">
+        <v>2.9794</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>-33031.018601968499</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="S15" s="9">
+        <v>3.5905</v>
+      </c>
+      <c r="T15" s="7">
+        <v>-35224.013096811497</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="V15" s="9">
+        <v>4.3269000000000002</v>
+      </c>
+      <c r="W15" s="7">
+        <v>-38109.451694342701</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>5.2270000000000003</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>-41915.713201084996</v>
+      </c>
+      <c r="AA15" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>6.4352999999999998</v>
+      </c>
+      <c r="AC15" s="7">
+        <v>-46987.7539499005</v>
+      </c>
+      <c r="AD15" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE15" s="9">
+        <v>8.1370000000000005</v>
+      </c>
+      <c r="AF15" s="7">
+        <v>-54043.980699610504</v>
+      </c>
+      <c r="AG15" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH15" s="9">
+        <v>10.703099999999999</v>
+      </c>
+      <c r="AI15" s="7">
+        <v>-64175.619448953803</v>
+      </c>
+      <c r="AJ15" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK15" s="9">
+        <v>14.136100000000001</v>
       </c>
     </row>
     <row r="16" spans="1:37">
       <c r="A16">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B16" s="3">
+        <v>-33130.425670696401</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2.0364</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-33099.287229644098</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="11">
+        <v>2.0364</v>
+      </c>
+      <c r="H16" s="3">
+        <v>-32766.596500830499</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="11">
+        <v>2.0364</v>
+      </c>
+      <c r="K16" s="3">
+        <v>-30692.553262151301</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M16" s="11">
+        <v>2.0491999999999999</v>
+      </c>
+      <c r="N16" s="15">
+        <v>-30337.915095195502</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="P16" s="11">
+        <v>2.9157999999999999</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>-31108.604969304499</v>
+      </c>
+      <c r="R16" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="S16" s="11">
+        <v>3.3176000000000001</v>
+      </c>
+      <c r="T16" s="3">
+        <v>-32080.7257213751</v>
+      </c>
+      <c r="U16" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="V16" s="11">
+        <v>3.8355999999999999</v>
+      </c>
+      <c r="W16" s="3">
+        <v>-33286.531116806</v>
+      </c>
+      <c r="X16" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y16" s="11">
+        <v>4.4470000000000001</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>-34811.612763867699</v>
+      </c>
+      <c r="AA16" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>5.1853999999999996</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>-36805.443227141201</v>
+      </c>
+      <c r="AD16" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE16" s="11">
+        <v>6.1836000000000002</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>-39549.583250622003</v>
+      </c>
+      <c r="AG16" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH16" s="11">
+        <v>7.6189999999999998</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>-43610.411867398703</v>
+      </c>
+      <c r="AJ16" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK16" s="11">
+        <v>10.117800000000001</v>
       </c>
     </row>
     <row r="17" spans="1:37">
       <c r="A17">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
+        <v>-30006.5654456267</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="11">
+        <v>2.0979999999999999</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-30005.642519869099</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="11">
+        <v>2.0960000000000001</v>
+      </c>
+      <c r="H17" s="3">
+        <v>-29997.049228332398</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J17" s="11">
+        <v>2.0990000000000002</v>
+      </c>
+      <c r="K17" s="3">
+        <v>-29899.606784187799</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="M17" s="11">
+        <v>2.1019999999999999</v>
+      </c>
+      <c r="N17" s="15">
+        <v>-29732.097531540399</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="P17" s="11">
+        <v>2.863</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>-29847.108572463902</v>
+      </c>
+      <c r="R17" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="S17" s="11">
+        <v>3.0760000000000001</v>
+      </c>
+      <c r="T17" s="3">
+        <v>-30016.0816244214</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="V17" s="11">
+        <v>3.4079999999999999</v>
+      </c>
+      <c r="W17" s="3">
+        <v>-30230.451275963798</v>
+      </c>
+      <c r="X17" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y17" s="11">
+        <v>3.843</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>-30500.868250021002</v>
+      </c>
+      <c r="AA17" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB17" s="11">
+        <v>4.3070000000000004</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>-30853.047829463801</v>
+      </c>
+      <c r="AD17" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE17" s="11">
+        <v>4.9859999999999998</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>-31341.425339437599</v>
+      </c>
+      <c r="AG17" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH17" s="11">
+        <v>6.0279999999999996</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>-32097.392712773599</v>
+      </c>
+      <c r="AJ17" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK17" s="11">
+        <v>7.9219999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:37">
       <c r="A18">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="3">
+        <v>-29544.8977501177</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2.5049999999999999</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-29544.898006627202</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="15">
+        <v>-29544.8998643349</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="J18" s="11">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="K18" s="3">
+        <v>-29545.229870776398</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" s="11">
+        <v>2.5150000000000001</v>
+      </c>
+      <c r="N18" s="3">
+        <v>-29565.382730330501</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="P18" s="11">
+        <v>3.17</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>-29594.220794238099</v>
+      </c>
+      <c r="R18" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="S18" s="11">
+        <v>3.355</v>
+      </c>
+      <c r="T18" s="3">
+        <v>-29627.906490169898</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="V18" s="11">
+        <v>3.66</v>
+      </c>
+      <c r="W18" s="3">
+        <v>-29668.682544006198</v>
+      </c>
+      <c r="X18" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y18" s="11">
+        <v>4.04</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>-29720.0741491136</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB18" s="11">
+        <v>4.4749999999999996</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>-29787.760254697499</v>
+      </c>
+      <c r="AD18" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE18" s="11">
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>-29882.556397666402</v>
+      </c>
+      <c r="AG18" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH18" s="11">
+        <v>6.0350000000000001</v>
+      </c>
+      <c r="AI18" s="3">
+        <v>-30029.4907166064</v>
+      </c>
+      <c r="AJ18" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="AK18" s="11">
+        <v>7.6950000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:37">
       <c r="A19">
-        <v>1000</v>
+        <v>100</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-29554.462376425101</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2.95</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-29554.4598071539</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G19" s="11">
+        <v>2.94</v>
+      </c>
+      <c r="H19" s="3">
+        <v>-29554.4359079571</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="J19" s="11">
+        <v>2.97</v>
+      </c>
+      <c r="K19" s="15">
+        <v>-29554.274247921599</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="M19" s="11">
+        <v>2.95</v>
+      </c>
+      <c r="N19" s="3">
+        <v>-29559.304305355599</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="P19" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>-29570.895034482699</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="S19" s="11">
+        <v>3.73</v>
+      </c>
+      <c r="T19" s="3">
+        <v>-29585.842300734701</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="V19" s="11">
+        <v>4.04</v>
+      </c>
+      <c r="W19" s="3">
+        <v>-29604.692872584499</v>
+      </c>
+      <c r="X19" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y19" s="11">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>-29628.720284272698</v>
+      </c>
+      <c r="AA19" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="AB19" s="11">
+        <v>4.93</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>-29660.509851340499</v>
+      </c>
+      <c r="AD19" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE19" s="11">
+        <v>5.59</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>-29705.3177032003</v>
+      </c>
+      <c r="AG19" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="AH19" s="11">
+        <v>6.49</v>
+      </c>
+      <c r="AI19" s="3">
+        <v>-29775.499596626101</v>
+      </c>
+      <c r="AJ19" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="AK19" s="11">
+        <v>8.2200000000000006</v>
       </c>
     </row>
     <row r="20" spans="1:37">
       <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20" s="3">
+        <v>-29547.518756825699</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="11">
+        <v>12.1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-29547.518749239902</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="G20" s="11">
+        <v>12.1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>-29547.518136943301</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="J20" s="11">
+        <v>12.1</v>
+      </c>
+      <c r="K20" s="15">
+        <v>-29547.515048455101</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="M20" s="11">
+        <v>12.1</v>
+      </c>
+      <c r="N20" s="3">
+        <v>-29547.554711811299</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="P20" s="11">
+        <v>12.1</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>-29547.799930458001</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="S20" s="11">
+        <v>12.3</v>
+      </c>
+      <c r="T20" s="3">
+        <v>-29548.368394974899</v>
+      </c>
+      <c r="U20" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="V20" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="W20" s="3">
+        <v>-29549.465232274699</v>
+      </c>
+      <c r="X20" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y20" s="11">
+        <v>12.6</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>-29551.1781055174</v>
+      </c>
+      <c r="AA20" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB20" s="11">
+        <v>13.1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>-29553.693657124699</v>
+      </c>
+      <c r="AD20" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE20" s="11">
+        <v>13.6</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>-29557.406549360399</v>
+      </c>
+      <c r="AG20" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="AH20" s="11">
+        <v>14.2</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>-29563.392167631198</v>
+      </c>
+      <c r="AJ20" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK20" s="11">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21">
         <v>5000</v>
       </c>
-    </row>
-    <row r="21" spans="1:37">
-      <c r="A21" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="5"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
-      <c r="AG21" s="5"/>
-      <c r="AH21" s="5"/>
-      <c r="AI21" s="5"/>
-      <c r="AJ21" s="5"/>
-      <c r="AK21" s="5"/>
+      <c r="B21" s="3">
+        <v>-29544.532875302499</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-29544.532868276801</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="G21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="H21" s="3">
+        <v>-29544.532757177301</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="J21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>-29544.532012605399</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="M21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="N21" s="15">
+        <v>-29544.529695282399</v>
+      </c>
+      <c r="O21" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="P21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>-29544.539163791</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="S21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="T21" s="3">
+        <v>-29544.566485219701</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="V21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="W21" s="3">
+        <v>-29544.620032941399</v>
+      </c>
+      <c r="X21" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y21" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>-29544.713852904901</v>
+      </c>
+      <c r="AA21" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB21" s="11">
+        <v>53</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>-29544.8731166131</v>
+      </c>
+      <c r="AD21" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="AE21" s="11">
+        <v>53.5</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>-29545.147965666802</v>
+      </c>
+      <c r="AG21" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH21" s="11">
+        <v>54</v>
+      </c>
+      <c r="AI21" s="3">
+        <v>-29545.657126957201</v>
+      </c>
+      <c r="AJ21" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="AK21" s="11">
+        <v>55.5</v>
+      </c>
     </row>
     <row r="22" spans="1:37">
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="H22">
-        <v>0.999</v>
-      </c>
-      <c r="K22">
-        <v>0.99</v>
-      </c>
-      <c r="N22">
-        <v>0.9</v>
-      </c>
-      <c r="Q22">
-        <v>0.8</v>
-      </c>
-      <c r="T22">
-        <v>0.7</v>
-      </c>
-      <c r="W22">
-        <v>0.6</v>
-      </c>
-      <c r="Z22">
-        <v>0.5</v>
-      </c>
-      <c r="AC22">
-        <v>0.4</v>
-      </c>
-      <c r="AF22">
-        <v>0.3</v>
-      </c>
-      <c r="AI22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37">
-      <c r="A24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37">
-      <c r="A25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37">
-      <c r="A26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:37">
-      <c r="A27">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:37">
-      <c r="A28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:37">
-      <c r="A29">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:37">
-      <c r="A30">
-        <v>5000</v>
+      <c r="A22">
+        <v>10000</v>
+      </c>
+      <c r="B22" s="16">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" s="14">
+        <v>106</v>
+      </c>
+      <c r="E22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="G22" s="14">
+        <v>106</v>
+      </c>
+      <c r="H22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="J22" s="14">
+        <v>106</v>
+      </c>
+      <c r="K22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="M22" s="14">
+        <v>106</v>
+      </c>
+      <c r="N22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="P22" s="14">
+        <v>106</v>
+      </c>
+      <c r="Q22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="S22" s="14">
+        <v>106</v>
+      </c>
+      <c r="T22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="U22" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="V22" s="14">
+        <v>106</v>
+      </c>
+      <c r="W22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="X22" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y22" s="14">
+        <v>106</v>
+      </c>
+      <c r="Z22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="AA22" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB22" s="14">
+        <v>106</v>
+      </c>
+      <c r="AC22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="AD22" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE22" s="14">
+        <v>106</v>
+      </c>
+      <c r="AF22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="AG22" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH22" s="14">
+        <v>106</v>
+      </c>
+      <c r="AI22" s="12">
+        <v>-29544.390834792001</v>
+      </c>
+      <c r="AJ22" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="AK22" s="14">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:AK1"/>
-    <mergeCell ref="A11:AK11"/>
-    <mergeCell ref="A21:AK21"/>
+    <mergeCell ref="A12:AK12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>